<commit_message>
add HEAD checking for updating date; fix newjersey and texas data
</commit_message>
<xml_diff>
--- a/data/2020-05-08/texas.xlsx
+++ b/data/2020-05-08/texas.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CHS-AAU\Epi\Covid\For Ektron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{67BBBD37-8D2A-4857-B231-F1DFAAC71579}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{77324211-5F25-4956-96BA-79E9DCC822CB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17900" windowHeight="10990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Case and Fatalities" sheetId="1" r:id="rId1"/>
     <sheet name="Trends" sheetId="2" r:id="rId2"/>
-    <sheet name="Recoveries" sheetId="4" r:id="rId3"/>
-    <sheet name="RecoveredActive by County" sheetId="5" r:id="rId4"/>
-    <sheet name="Tests" sheetId="6" r:id="rId5"/>
-    <sheet name="Testing Trends" sheetId="3" r:id="rId6"/>
+    <sheet name="Recoveries" sheetId="3" r:id="rId3"/>
+    <sheet name="RecoveredActive by County" sheetId="4" r:id="rId4"/>
+    <sheet name="Tests by day" sheetId="5" r:id="rId5"/>
+    <sheet name="Tests" sheetId="6" r:id="rId6"/>
     <sheet name="Hospitalizations" sheetId="7" r:id="rId7"/>
     <sheet name="Cases by Age Group" sheetId="8" r:id="rId8"/>
     <sheet name="Cases by Gender" sheetId="9" r:id="rId9"/>
@@ -32,9 +32,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="320">
-  <si>
-    <t>COVID-19 Positive Cases and Fatalities by County as of 5/07 at 10:45AM CST</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="322">
+  <si>
+    <t>COVID-19 Positive Cases and Fatalities by County as of 5/08 at 10:45AM CST</t>
   </si>
   <si>
     <t>County</t>
@@ -811,7 +811,7 @@
     <t>Total</t>
   </si>
   <si>
-    <t>COVID-19 Positive Cases and Fatalities over Time as of 5/07 at 10:45AM CST</t>
+    <t>COVID-19 Positive Cases and Fatalities over Time as of 5/08 at 10:45AM CST</t>
   </si>
   <si>
     <t>Date</t>
@@ -835,10 +835,7 @@
 Fatalities</t>
   </si>
   <si>
-    <t>Testing and Positivity Rate over Time as of 5/07 at 10:45AM CST</t>
-  </si>
-  <si>
-    <t>Estimated Number of People Recovered from and Active Cases of SARS-CoV-2 as of 5/07 at 9:30AM CST</t>
+    <t>Estimated Number of People Recovered from and Active Cases of SARS-CoV-2 as of 5/08 at 9:30AM CST</t>
   </si>
   <si>
     <t>Recovered</t>
@@ -850,10 +847,21 @@
     <t>This number is an estimate based on several assumptions related to hospitalization rates and recovery times, which were informed by data available to date. These assumptions are subject to change as we learn more about COVID-19. The estimated number does not include data from any cases reported prior to 3/24/2020.</t>
   </si>
   <si>
-    <t>Estimated Number of People Recovered from and Active Cases of SARS-CoV-2 by County as of 5/06 at 9:30AM CST</t>
-  </si>
-  <si>
-    <t>Number of People Tested for SARS-CoV-2 in Texas as of 5/07 at 9:30AM CST</t>
+    <t>Estimated Number of People Recovered from and Active Cases of SARS-CoV-2 by County as of 5/07 at 9:30AM CST</t>
+  </si>
+  <si>
+    <t>Testing and Positivity Rate over Time as of 5/08 at 10:45AM CST</t>
+  </si>
+  <si>
+    <t>Total
+Tests
+reported</t>
+  </si>
+  <si>
+    <t>Tests include those performed by public labs (Laboratory Response Network) and private labs (commercial labs, hospitals, physician offices, and drive-thru sites) reported electronically and non-electronically to DSHS.</t>
+  </si>
+  <si>
+    <t>Number of People Tested for SARS-CoV-2 in Texas as of 5/08 at 9:30AM CST</t>
   </si>
   <si>
     <t>Location</t>
@@ -868,10 +876,13 @@
     <t>No. Tests by Commercial labs*</t>
   </si>
   <si>
+    <t>Total Tests</t>
+  </si>
+  <si>
     <t>*Unable to deduplicate figures for Commercial labs.</t>
   </si>
   <si>
-    <t>Texas Statewide Hospitalization Data as of 5/07 at 9:30AM CST</t>
+    <t>Texas Statewide Hospitalization Data as of 5/08 at 9:30AM CST</t>
   </si>
   <si>
     <t>Hospital data</t>
@@ -892,7 +903,7 @@
     <t>Available Texas Ventilators</t>
   </si>
   <si>
-    <t>Age of Confirmed Cases as of 5/07 at 9:30 AM CST</t>
+    <t>Age of Confirmed Cases as of 5/08 at 9:30 AM CST</t>
   </si>
   <si>
     <t>Age
@@ -947,10 +958,10 @@
     <t>Demographic data comes from completed case investigations by local and regional health departments received by DSHS.</t>
   </si>
   <si>
-    <t>Completed case investigations received by DSHS =          12,533</t>
-  </si>
-  <si>
-    <t>Gender of Confirmed Cases as of 5/07 at 9:30 AM CST</t>
+    <t>Completed case investigations received by DSHS =          12,927</t>
+  </si>
+  <si>
+    <t>Gender of Confirmed Cases as of 5/08 at 9:30 AM CST</t>
   </si>
   <si>
     <t>Gender</t>
@@ -962,7 +973,7 @@
     <t>Male</t>
   </si>
   <si>
-    <t>Race/Ethnicity of Confirmed Cases as of 5/07 at 9:30 AM CST</t>
+    <t>Race/Ethnicity of Confirmed Cases as of 5/08 at 9:30 AM CST</t>
   </si>
   <si>
     <t>Race/Ethnicity</t>
@@ -983,21 +994,16 @@
     <t>White</t>
   </si>
   <si>
-    <t>Age of Confirmed Fatalities as of 5/07 at 9:30 AM CST</t>
-  </si>
-  <si>
-    <t>Completed investigations received by DSHS =          449</t>
-  </si>
-  <si>
-    <t>Gender of Confirmed Fatalities as of 5/07 at 9:30 AM CST</t>
-  </si>
-  <si>
-    <t>Race/Ethnicity of Confirmed Fatalities as of 5/07 at 9:30 AM CST</t>
-  </si>
-  <si>
-    <t>Total
-Tests
-Reported</t>
+    <t>Age of Confirmed Fatalities as of 5/08 at 9:30 AM CST</t>
+  </si>
+  <si>
+    <t>Completed investigations received by DSHS =          453</t>
+  </si>
+  <si>
+    <t>Gender of Confirmed Fatalities as of 5/08 at 9:30 AM CST</t>
+  </si>
+  <si>
+    <t>Race/Ethnicity of Confirmed Fatalities as of 5/08 at 9:30 AM CST</t>
   </si>
   <si>
     <t>COVID-19
@@ -1008,16 +1014,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="###,##0"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="166" formatCode="##,###,##0"/>
-    <numFmt numFmtId="167" formatCode="###,###,###,###,##0"/>
-    <numFmt numFmtId="168" formatCode="##0"/>
-    <numFmt numFmtId="169" formatCode="##########.00&quot;%&quot;_);\(##########.00&quot;%&quot;\)"/>
-    <numFmt numFmtId="170" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="###,###,###,###,##0"/>
+    <numFmt numFmtId="170" formatCode="##0"/>
+    <numFmt numFmtId="172" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="9.5"/>
       <color rgb="FF000000"/>
@@ -1039,6 +1044,13 @@
       <sz val="9.5"/>
       <color rgb="FF112277"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.5"/>
+      <color rgb="FF112277"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1109,7 +1121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1137,17 +1149,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="168" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="170" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1157,6 +1166,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1295,7 +1310,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1306,11 +1321,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1328,7 +1343,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3" s="4">
         <v>0</v>
@@ -1350,7 +1365,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="4">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C5" s="4">
         <v>0</v>
@@ -1438,7 +1453,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="4">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C13" s="4">
         <v>2</v>
@@ -1471,7 +1486,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="4">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="C16" s="4">
         <v>3</v>
@@ -1482,10 +1497,10 @@
         <v>18</v>
       </c>
       <c r="B17" s="4">
-        <v>1761</v>
+        <v>1805</v>
       </c>
       <c r="C17" s="4">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -1537,10 +1552,10 @@
         <v>23</v>
       </c>
       <c r="B22" s="4">
-        <v>588</v>
+        <v>613</v>
       </c>
       <c r="C22" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -1548,7 +1563,7 @@
         <v>24</v>
       </c>
       <c r="B23" s="4">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="C23" s="4">
         <v>17</v>
@@ -1603,7 +1618,7 @@
         <v>29</v>
       </c>
       <c r="B28" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C28" s="4">
         <v>0</v>
@@ -1614,7 +1629,7 @@
         <v>30</v>
       </c>
       <c r="B29" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C29" s="4">
         <v>0</v>
@@ -1636,7 +1651,7 @@
         <v>32</v>
       </c>
       <c r="B31" s="4">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C31" s="4">
         <v>3</v>
@@ -1647,7 +1662,7 @@
         <v>33</v>
       </c>
       <c r="B32" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C32" s="4">
         <v>1</v>
@@ -1658,10 +1673,10 @@
         <v>34</v>
       </c>
       <c r="B33" s="4">
-        <v>469</v>
+        <v>483</v>
       </c>
       <c r="C33" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -1724,7 +1739,7 @@
         <v>40</v>
       </c>
       <c r="B39" s="4">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C39" s="4">
         <v>1</v>
@@ -1790,10 +1805,10 @@
         <v>46</v>
       </c>
       <c r="B45" s="4">
-        <v>839</v>
+        <v>857</v>
       </c>
       <c r="C45" s="4">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -1812,7 +1827,7 @@
         <v>48</v>
       </c>
       <c r="B47" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C47" s="4">
         <v>0</v>
@@ -1823,7 +1838,7 @@
         <v>49</v>
       </c>
       <c r="B48" s="4">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C48" s="4">
         <v>6</v>
@@ -1867,7 +1882,7 @@
         <v>53</v>
       </c>
       <c r="B52" s="4">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C52" s="4">
         <v>2</v>
@@ -1933,7 +1948,7 @@
         <v>59</v>
       </c>
       <c r="B58" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C58" s="4">
         <v>0</v>
@@ -1944,10 +1959,10 @@
         <v>60</v>
       </c>
       <c r="B59" s="4">
-        <v>4869</v>
+        <v>5120</v>
       </c>
       <c r="C59" s="4">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -1977,7 +1992,7 @@
         <v>63</v>
       </c>
       <c r="B62" s="4">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C62" s="4">
         <v>0</v>
@@ -1999,10 +2014,10 @@
         <v>65</v>
       </c>
       <c r="B64" s="4">
-        <v>846</v>
+        <v>872</v>
       </c>
       <c r="C64" s="4">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -2065,7 +2080,7 @@
         <v>71</v>
       </c>
       <c r="B70" s="4">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C70" s="4">
         <v>4</v>
@@ -2087,10 +2102,10 @@
         <v>73</v>
       </c>
       <c r="B72" s="4">
-        <v>1119</v>
+        <v>1190</v>
       </c>
       <c r="C72" s="4">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -2098,10 +2113,10 @@
         <v>74</v>
       </c>
       <c r="B73" s="4">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="C73" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -2109,7 +2124,7 @@
         <v>75</v>
       </c>
       <c r="B74" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C74" s="4">
         <v>1</v>
@@ -2142,7 +2157,7 @@
         <v>78</v>
       </c>
       <c r="B77" s="4">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C77" s="4">
         <v>1</v>
@@ -2186,10 +2201,10 @@
         <v>82</v>
       </c>
       <c r="B81" s="4">
-        <v>1287</v>
+        <v>1332</v>
       </c>
       <c r="C81" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -2241,7 +2256,7 @@
         <v>87</v>
       </c>
       <c r="B86" s="4">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="C86" s="4">
         <v>28</v>
@@ -2318,7 +2333,7 @@
         <v>94</v>
       </c>
       <c r="B93" s="4">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="C93" s="4">
         <v>0</v>
@@ -2329,7 +2344,7 @@
         <v>95</v>
       </c>
       <c r="B94" s="4">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="C94" s="4">
         <v>0</v>
@@ -2340,7 +2355,7 @@
         <v>96</v>
       </c>
       <c r="B95" s="4">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C95" s="4">
         <v>1</v>
@@ -2351,7 +2366,7 @@
         <v>97</v>
       </c>
       <c r="B96" s="4">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C96" s="4">
         <v>0</v>
@@ -2384,7 +2399,7 @@
         <v>100</v>
       </c>
       <c r="B99" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C99" s="4">
         <v>0</v>
@@ -2395,7 +2410,7 @@
         <v>101</v>
       </c>
       <c r="B100" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C100" s="4">
         <v>2</v>
@@ -2428,10 +2443,10 @@
         <v>104</v>
       </c>
       <c r="B103" s="4">
-        <v>7244</v>
+        <v>7377</v>
       </c>
       <c r="C103" s="4">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -2439,7 +2454,7 @@
         <v>105</v>
       </c>
       <c r="B104" s="4">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="C104" s="4">
         <v>6</v>
@@ -2472,7 +2487,7 @@
         <v>108</v>
       </c>
       <c r="B107" s="4">
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="C107" s="4">
         <v>1</v>
@@ -2494,7 +2509,7 @@
         <v>110</v>
       </c>
       <c r="B109" s="4">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C109" s="4">
         <v>0</v>
@@ -2505,7 +2520,7 @@
         <v>111</v>
       </c>
       <c r="B110" s="4">
-        <v>359</v>
+        <v>368</v>
       </c>
       <c r="C110" s="4">
         <v>7</v>
@@ -2516,7 +2531,7 @@
         <v>112</v>
       </c>
       <c r="B111" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C111" s="4">
         <v>1</v>
@@ -2527,7 +2542,7 @@
         <v>113</v>
       </c>
       <c r="B112" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C112" s="4">
         <v>1</v>
@@ -2593,7 +2608,7 @@
         <v>119</v>
       </c>
       <c r="B118" s="4">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C118" s="4">
         <v>3</v>
@@ -2648,7 +2663,7 @@
         <v>124</v>
       </c>
       <c r="B123" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C123" s="4">
         <v>1</v>
@@ -2670,10 +2685,10 @@
         <v>126</v>
       </c>
       <c r="B125" s="4">
-        <v>336</v>
+        <v>353</v>
       </c>
       <c r="C125" s="4">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -2703,7 +2718,7 @@
         <v>129</v>
       </c>
       <c r="B128" s="4">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C128" s="4">
         <v>4</v>
@@ -2714,7 +2729,7 @@
         <v>130</v>
       </c>
       <c r="B129" s="4">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C129" s="4">
         <v>0</v>
@@ -2736,7 +2751,7 @@
         <v>132</v>
       </c>
       <c r="B131" s="4">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C131" s="4">
         <v>1</v>
@@ -2780,7 +2795,7 @@
         <v>136</v>
       </c>
       <c r="B135" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C135" s="4">
         <v>0</v>
@@ -2791,7 +2806,7 @@
         <v>137</v>
       </c>
       <c r="B136" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C136" s="4">
         <v>0</v>
@@ -2857,7 +2872,7 @@
         <v>143</v>
       </c>
       <c r="B142" s="4">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C142" s="4">
         <v>0</v>
@@ -2901,7 +2916,7 @@
         <v>147</v>
       </c>
       <c r="B146" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C146" s="4">
         <v>0</v>
@@ -2912,7 +2927,7 @@
         <v>148</v>
       </c>
       <c r="B147" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C147" s="4">
         <v>0</v>
@@ -2923,7 +2938,7 @@
         <v>149</v>
       </c>
       <c r="B148" s="4">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C148" s="4">
         <v>1</v>
@@ -2989,10 +3004,10 @@
         <v>155</v>
       </c>
       <c r="B154" s="4">
-        <v>575</v>
+        <v>582</v>
       </c>
       <c r="C154" s="4">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -3011,7 +3026,7 @@
         <v>157</v>
       </c>
       <c r="B156" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C156" s="4">
         <v>0</v>
@@ -3022,7 +3037,7 @@
         <v>158</v>
       </c>
       <c r="B157" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C157" s="4">
         <v>0</v>
@@ -3088,7 +3103,7 @@
         <v>164</v>
       </c>
       <c r="B163" s="4">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C163" s="4">
         <v>4</v>
@@ -3110,7 +3125,7 @@
         <v>166</v>
       </c>
       <c r="B165" s="4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C165" s="4">
         <v>2</v>
@@ -3132,10 +3147,10 @@
         <v>168</v>
       </c>
       <c r="B167" s="4">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C167" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -3187,7 +3202,7 @@
         <v>173</v>
       </c>
       <c r="B172" s="4">
-        <v>672</v>
+        <v>689</v>
       </c>
       <c r="C172" s="4">
         <v>15</v>
@@ -3198,10 +3213,10 @@
         <v>174</v>
       </c>
       <c r="B173" s="4">
-        <v>454</v>
+        <v>487</v>
       </c>
       <c r="C173" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -3242,7 +3257,7 @@
         <v>178</v>
       </c>
       <c r="B177" s="4">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C177" s="4">
         <v>2</v>
@@ -3275,7 +3290,7 @@
         <v>181</v>
       </c>
       <c r="B180" s="4">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C180" s="4">
         <v>3</v>
@@ -3286,7 +3301,7 @@
         <v>182</v>
       </c>
       <c r="B181" s="4">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C181" s="4">
         <v>1</v>
@@ -3330,7 +3345,7 @@
         <v>186</v>
       </c>
       <c r="B185" s="4">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C185" s="4">
         <v>3</v>
@@ -3341,7 +3356,7 @@
         <v>187</v>
       </c>
       <c r="B186" s="4">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C186" s="4">
         <v>0</v>
@@ -3374,7 +3389,7 @@
         <v>190</v>
       </c>
       <c r="B189" s="4">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C189" s="4">
         <v>0</v>
@@ -3385,7 +3400,7 @@
         <v>191</v>
       </c>
       <c r="B190" s="4">
-        <v>971</v>
+        <v>1027</v>
       </c>
       <c r="C190" s="4">
         <v>15</v>
@@ -3418,7 +3433,7 @@
         <v>194</v>
       </c>
       <c r="B193" s="4">
-        <v>333</v>
+        <v>343</v>
       </c>
       <c r="C193" s="4">
         <v>3</v>
@@ -3451,7 +3466,7 @@
         <v>197</v>
       </c>
       <c r="B196" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C196" s="4">
         <v>0</v>
@@ -3462,7 +3477,7 @@
         <v>198</v>
       </c>
       <c r="B197" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C197" s="4">
         <v>0</v>
@@ -3506,10 +3521,10 @@
         <v>202</v>
       </c>
       <c r="B201" s="4">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C201" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -3627,7 +3642,7 @@
         <v>213</v>
       </c>
       <c r="B212" s="4">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C212" s="4">
         <v>4</v>
@@ -3638,7 +3653,7 @@
         <v>214</v>
       </c>
       <c r="B213" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C213" s="4">
         <v>0</v>
@@ -3649,7 +3664,7 @@
         <v>215</v>
       </c>
       <c r="B214" s="4">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C214" s="4">
         <v>3</v>
@@ -3671,7 +3686,7 @@
         <v>217</v>
       </c>
       <c r="B216" s="4">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C216" s="4">
         <v>0</v>
@@ -3737,10 +3752,10 @@
         <v>223</v>
       </c>
       <c r="B222" s="4">
-        <v>2813</v>
+        <v>2956</v>
       </c>
       <c r="C222" s="4">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -3748,7 +3763,7 @@
         <v>224</v>
       </c>
       <c r="B223" s="4">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C223" s="4">
         <v>6</v>
@@ -3792,7 +3807,7 @@
         <v>228</v>
       </c>
       <c r="B227" s="4">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C227" s="4">
         <v>0</v>
@@ -3803,7 +3818,7 @@
         <v>229</v>
       </c>
       <c r="B228" s="4">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C228" s="4">
         <v>1</v>
@@ -3814,10 +3829,10 @@
         <v>230</v>
       </c>
       <c r="B229" s="4">
-        <v>1946</v>
+        <v>2002</v>
       </c>
       <c r="C229" s="4">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -3825,7 +3840,7 @@
         <v>231</v>
       </c>
       <c r="B230" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C230" s="4">
         <v>0</v>
@@ -3847,7 +3862,7 @@
         <v>233</v>
       </c>
       <c r="B232" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C232" s="4">
         <v>0</v>
@@ -3913,7 +3928,7 @@
         <v>239</v>
       </c>
       <c r="B238" s="4">
-        <v>315</v>
+        <v>332</v>
       </c>
       <c r="C238" s="4">
         <v>2</v>
@@ -3924,7 +3939,7 @@
         <v>240</v>
       </c>
       <c r="B239" s="4">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C239" s="4">
         <v>0</v>
@@ -3946,7 +3961,7 @@
         <v>242</v>
       </c>
       <c r="B241" s="4">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C241" s="4">
         <v>18</v>
@@ -3957,7 +3972,7 @@
         <v>243</v>
       </c>
       <c r="B242" s="4">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="C242" s="4">
         <v>17</v>
@@ -3968,7 +3983,7 @@
         <v>244</v>
       </c>
       <c r="B243" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C243" s="4">
         <v>0</v>
@@ -3979,7 +3994,7 @@
         <v>245</v>
       </c>
       <c r="B244" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C244" s="4">
         <v>0</v>
@@ -3990,7 +4005,7 @@
         <v>246</v>
       </c>
       <c r="B245" s="4">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C245" s="4">
         <v>2</v>
@@ -4023,7 +4038,7 @@
         <v>249</v>
       </c>
       <c r="B248" s="4">
-        <v>341</v>
+        <v>352</v>
       </c>
       <c r="C248" s="4">
         <v>12</v>
@@ -4067,7 +4082,7 @@
         <v>253</v>
       </c>
       <c r="B252" s="4">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C252" s="4">
         <v>0</v>
@@ -4122,10 +4137,10 @@
         <v>258</v>
       </c>
       <c r="B257" s="4">
-        <v>35390</v>
+        <v>36609</v>
       </c>
       <c r="C257" s="4">
-        <v>973</v>
+        <v>1004</v>
       </c>
     </row>
   </sheetData>
@@ -4144,7 +4159,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2:XFD2"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4155,93 +4170,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>307</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="A1" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="B3" s="9">
-        <v>462</v>
-      </c>
-      <c r="C3" s="12">
+        <v>466</v>
+      </c>
+      <c r="C3" s="15">
         <f>B3/B$9</f>
-        <v>3.6862682518152078E-2</v>
+        <v>3.6048580490446354E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B4" s="9">
-        <v>1896</v>
-      </c>
-      <c r="C4" s="12">
+        <v>1981</v>
+      </c>
+      <c r="C4" s="15">
         <f t="shared" ref="C4:C9" si="0">B4/B$9</f>
-        <v>0.15128061916540333</v>
+        <v>0.15324514581882881</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="B5" s="9">
-        <v>4821</v>
-      </c>
-      <c r="C5" s="12">
+        <v>4820</v>
+      </c>
+      <c r="C5" s="15">
         <f t="shared" si="0"/>
-        <v>0.38466448575759993</v>
+        <v>0.37286299992264255</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B6" s="9">
-        <v>87</v>
-      </c>
-      <c r="C6" s="12">
+        <v>89</v>
+      </c>
+      <c r="C6" s="15">
         <f t="shared" si="0"/>
-        <v>6.9416739806909761E-3</v>
+        <v>6.8848147288620718E-3</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B7" s="9">
-        <v>3521</v>
-      </c>
-      <c r="C7" s="12">
+        <v>3734</v>
+      </c>
+      <c r="C7" s="15">
         <f t="shared" si="0"/>
-        <v>0.28093832282773479</v>
+        <v>0.28885278873675252</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B8" s="9">
-        <v>1746</v>
-      </c>
-      <c r="C8" s="12">
+        <v>1837</v>
+      </c>
+      <c r="C8" s="15">
         <f t="shared" si="0"/>
-        <v>0.13931221575041888</v>
+        <v>0.14210567030246771</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -4249,26 +4264,26 @@
         <v>258</v>
       </c>
       <c r="B9" s="9">
-        <v>12533</v>
-      </c>
-      <c r="C9" s="12">
+        <v>12927</v>
+      </c>
+      <c r="C9" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>301</v>
-      </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="A11" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
     </row>
     <row r="12" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
+      <c r="A12" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4288,188 +4303,188 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2:XFD2"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6328125" customWidth="1"/>
+    <col min="3" max="3" width="7.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>314</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="A1" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B3" s="10">
         <v>0</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="15">
         <f>B3/B$16</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B4" s="10">
         <v>0</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="15">
         <f t="shared" ref="C4:C16" si="0">B4/B$16</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B5" s="10">
         <v>2</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="15">
         <f t="shared" si="0"/>
-        <v>4.4543429844097994E-3</v>
+        <v>4.4150110375275938E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B6" s="10">
         <v>10</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="15">
         <f t="shared" si="0"/>
-        <v>2.2271714922048998E-2</v>
+        <v>2.2075055187637971E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B7" s="10">
         <v>9</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="15">
         <f t="shared" si="0"/>
-        <v>2.0044543429844099E-2</v>
+        <v>1.9867549668874173E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B8" s="10">
         <v>20</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="15">
         <f t="shared" si="0"/>
-        <v>4.4543429844097995E-2</v>
+        <v>4.4150110375275942E-2</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B9" s="10">
-        <v>46</v>
-      </c>
-      <c r="C9" s="12">
+        <v>47</v>
+      </c>
+      <c r="C9" s="15">
         <f t="shared" si="0"/>
-        <v>0.10244988864142539</v>
+        <v>0.10375275938189846</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B10" s="10">
-        <v>40</v>
-      </c>
-      <c r="C10" s="12">
+        <v>41</v>
+      </c>
+      <c r="C10" s="15">
         <f t="shared" si="0"/>
-        <v>8.9086859688195991E-2</v>
+        <v>9.0507726269315678E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B11" s="10">
         <v>57</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="15">
         <f t="shared" si="0"/>
-        <v>0.12694877505567928</v>
+        <v>0.12582781456953643</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="B12" s="10">
-        <v>41</v>
-      </c>
-      <c r="C12" s="12">
+        <v>43</v>
+      </c>
+      <c r="C12" s="15">
         <f t="shared" si="0"/>
-        <v>9.1314031180400893E-2</v>
+        <v>9.4922737306843266E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="B13" s="10">
         <v>42</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="15">
         <f t="shared" si="0"/>
-        <v>9.3541202672605794E-2</v>
+        <v>9.2715231788079472E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B14" s="10">
         <v>180</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="15">
         <f t="shared" si="0"/>
-        <v>0.40089086859688194</v>
+        <v>0.39735099337748342</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B15" s="10">
         <v>2</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="15">
         <f t="shared" si="0"/>
-        <v>4.4543429844097994E-3</v>
+        <v>4.4150110375275938E-3</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -4477,26 +4492,26 @@
         <v>258</v>
       </c>
       <c r="B16" s="10">
-        <v>449</v>
-      </c>
-      <c r="C16" s="12">
+        <v>453</v>
+      </c>
+      <c r="C16" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
-        <v>301</v>
-      </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
+      <c r="A18" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
     </row>
     <row r="19" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>315</v>
-      </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
+      <c r="A19" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4516,68 +4531,68 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2:XFD2"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1796875" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>316</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="A1" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B3" s="10">
         <v>179</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="15">
         <f>B3/B$6</f>
-        <v>0.39866369710467708</v>
+        <v>0.39514348785871967</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="B4" s="10">
-        <v>238</v>
-      </c>
-      <c r="C4" s="12">
+        <v>242</v>
+      </c>
+      <c r="C4" s="15">
         <f t="shared" ref="C4:C6" si="0">B4/B$6</f>
-        <v>0.53006681514476617</v>
+        <v>0.5342163355408388</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B5" s="10">
         <v>32</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="15">
         <f t="shared" si="0"/>
-        <v>7.126948775055679E-2</v>
+        <v>7.0640176600441501E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -4585,26 +4600,26 @@
         <v>258</v>
       </c>
       <c r="B6" s="10">
-        <v>449</v>
-      </c>
-      <c r="C6" s="12">
+        <v>453</v>
+      </c>
+      <c r="C6" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>301</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
+      <c r="A8" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
     </row>
     <row r="9" spans="1:3" ht="43" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>315</v>
-      </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
+      <c r="A9" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4624,104 +4639,104 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2:XFD2"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.26953125" customWidth="1"/>
+    <col min="3" max="3" width="7.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="A1" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="B3" s="10">
         <v>6</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="15">
         <f>B3/B$9</f>
-        <v>1.3363028953229399E-2</v>
+        <v>1.3245033112582781E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B4" s="10">
-        <v>61</v>
-      </c>
-      <c r="C4" s="12">
+        <v>62</v>
+      </c>
+      <c r="C4" s="15">
         <f t="shared" ref="C4:C9" si="0">B4/B$9</f>
-        <v>0.13585746102449889</v>
+        <v>0.13686534216335541</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="B5" s="10">
         <v>99</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="15">
         <f t="shared" si="0"/>
-        <v>0.22048997772828507</v>
+        <v>0.2185430463576159</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B6" s="10">
-        <v>2</v>
-      </c>
-      <c r="C6" s="12">
+        <v>1</v>
+      </c>
+      <c r="C6" s="15">
         <f t="shared" si="0"/>
-        <v>4.4543429844097994E-3</v>
+        <v>2.2075055187637969E-3</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B7" s="10">
-        <v>167</v>
-      </c>
-      <c r="C7" s="12">
+        <v>170</v>
+      </c>
+      <c r="C7" s="15">
         <f t="shared" si="0"/>
-        <v>0.37193763919821826</v>
+        <v>0.37527593818984545</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B8" s="10">
-        <v>114</v>
-      </c>
-      <c r="C8" s="12">
+        <v>115</v>
+      </c>
+      <c r="C8" s="15">
         <f t="shared" si="0"/>
-        <v>0.25389755011135856</v>
+        <v>0.25386313465783666</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -4729,26 +4744,26 @@
         <v>258</v>
       </c>
       <c r="B9" s="10">
-        <v>449</v>
-      </c>
-      <c r="C9" s="12">
+        <v>453</v>
+      </c>
+      <c r="C9" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>301</v>
-      </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="A11" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
     </row>
     <row r="12" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>315</v>
-      </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
+      <c r="A12" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4763,7 +4778,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4780,13 +4795,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" ht="43" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -5891,6 +5906,23 @@
       </c>
       <c r="E66" s="4">
         <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="6">
+        <v>43959</v>
+      </c>
+      <c r="B67" s="4">
+        <v>36609</v>
+      </c>
+      <c r="C67" s="4">
+        <v>1004</v>
+      </c>
+      <c r="D67" s="4">
+        <v>1219</v>
+      </c>
+      <c r="E67" s="4">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -5903,7 +5935,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -5919,32 +5951,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="101" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="B1" s="14"/>
+      <c r="A1" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
-        <v>18440</v>
+        <v>19197</v>
       </c>
       <c r="B3" s="7">
-        <v>15977</v>
+        <v>16408</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="218" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="B5" s="14"/>
+      <c r="A5" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="B5" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5957,13 +5989,13 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C258"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2:XFD2"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5974,21 +6006,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="A1" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -5999,7 +6031,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="4">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6007,10 +6039,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6021,7 +6053,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="4">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6065,7 +6097,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6073,10 +6105,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6106,10 +6138,10 @@
         <v>14</v>
       </c>
       <c r="B13" s="4">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C13" s="4">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6128,10 +6160,10 @@
         <v>16</v>
       </c>
       <c r="B15" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C15" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6142,7 +6174,7 @@
         <v>123</v>
       </c>
       <c r="C16" s="4">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6150,10 +6182,10 @@
         <v>18</v>
       </c>
       <c r="B17" s="4">
-        <v>834</v>
+        <v>867</v>
       </c>
       <c r="C17" s="4">
-        <v>791</v>
+        <v>841</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6205,10 +6237,10 @@
         <v>23</v>
       </c>
       <c r="B22" s="4">
-        <v>303</v>
+        <v>319</v>
       </c>
       <c r="C22" s="4">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6216,10 +6248,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="4">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C23" s="4">
-        <v>84</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6260,10 +6292,10 @@
         <v>28</v>
       </c>
       <c r="B27" s="4">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C27" s="4">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6271,10 +6303,10 @@
         <v>29</v>
       </c>
       <c r="B28" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C28" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6282,10 +6314,10 @@
         <v>30</v>
       </c>
       <c r="B29" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C29" s="4">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6293,7 +6325,7 @@
         <v>31</v>
       </c>
       <c r="B30" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C30" s="4">
         <v>19</v>
@@ -6304,10 +6336,10 @@
         <v>32</v>
       </c>
       <c r="B31" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C31" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6318,7 +6350,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6326,10 +6358,10 @@
         <v>34</v>
       </c>
       <c r="B33" s="4">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="C33" s="4">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6373,7 +6405,7 @@
         <v>11</v>
       </c>
       <c r="C37" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6381,10 +6413,10 @@
         <v>39</v>
       </c>
       <c r="B38" s="4">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C38" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6425,10 +6457,10 @@
         <v>43</v>
       </c>
       <c r="B42" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C42" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6450,7 +6482,7 @@
         <v>0</v>
       </c>
       <c r="C44" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6458,10 +6490,10 @@
         <v>46</v>
       </c>
       <c r="B45" s="4">
-        <v>557</v>
+        <v>569</v>
       </c>
       <c r="C45" s="4">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6494,7 +6526,7 @@
         <v>44</v>
       </c>
       <c r="C48" s="4">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6535,10 +6567,10 @@
         <v>53</v>
       </c>
       <c r="B52" s="4">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C52" s="4">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6612,10 +6644,10 @@
         <v>60</v>
       </c>
       <c r="B59" s="4">
-        <v>2211</v>
+        <v>2294</v>
       </c>
       <c r="C59" s="4">
-        <v>2291</v>
+        <v>2452</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6623,10 +6655,10 @@
         <v>61</v>
       </c>
       <c r="B60" s="4">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C60" s="4">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6634,10 +6666,10 @@
         <v>63</v>
       </c>
       <c r="B61" s="4">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C61" s="4">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6656,10 +6688,10 @@
         <v>65</v>
       </c>
       <c r="B63" s="4">
-        <v>406</v>
+        <v>421</v>
       </c>
       <c r="C63" s="4">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6700,10 +6732,10 @@
         <v>68</v>
       </c>
       <c r="B67" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C67" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6736,7 +6768,7 @@
         <v>63</v>
       </c>
       <c r="C70" s="4">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6755,10 +6787,10 @@
         <v>74</v>
       </c>
       <c r="B72" s="4">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C72" s="4">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6766,10 +6798,10 @@
         <v>73</v>
       </c>
       <c r="B73" s="4">
-        <v>559</v>
+        <v>619</v>
       </c>
       <c r="C73" s="4">
-        <v>499</v>
+        <v>477</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6780,7 +6812,7 @@
         <v>10</v>
       </c>
       <c r="C74" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6799,7 +6831,7 @@
         <v>77</v>
       </c>
       <c r="B76" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C76" s="4">
         <v>11</v>
@@ -6813,7 +6845,7 @@
         <v>9</v>
       </c>
       <c r="C77" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6854,10 +6886,10 @@
         <v>82</v>
       </c>
       <c r="B81" s="4">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C81" s="4">
-        <v>1008</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6890,7 +6922,7 @@
         <v>1</v>
       </c>
       <c r="C84" s="4">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6909,10 +6941,10 @@
         <v>87</v>
       </c>
       <c r="B86" s="4">
-        <v>382</v>
+        <v>394</v>
       </c>
       <c r="C86" s="4">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6975,10 +7007,10 @@
         <v>93</v>
       </c>
       <c r="B92" s="4">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C92" s="4">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6986,10 +7018,10 @@
         <v>94</v>
       </c>
       <c r="B93" s="4">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C93" s="4">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -6997,7 +7029,7 @@
         <v>95</v>
       </c>
       <c r="B94" s="4">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C94" s="4">
         <v>62</v>
@@ -7019,10 +7051,10 @@
         <v>97</v>
       </c>
       <c r="B96" s="4">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C96" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7033,7 +7065,7 @@
         <v>18</v>
       </c>
       <c r="C97" s="4">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7052,10 +7084,10 @@
         <v>100</v>
       </c>
       <c r="B99" s="4">
+        <v>1</v>
+      </c>
+      <c r="C99" s="4">
         <v>4</v>
-      </c>
-      <c r="C99" s="4">
-        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7063,10 +7095,10 @@
         <v>101</v>
       </c>
       <c r="B100" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C100" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7085,10 +7117,10 @@
         <v>103</v>
       </c>
       <c r="B102" s="4">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C102" s="4">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7096,10 +7128,10 @@
         <v>104</v>
       </c>
       <c r="B103" s="4">
-        <v>2685</v>
+        <v>2779</v>
       </c>
       <c r="C103" s="4">
-        <v>4299</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7107,10 +7139,10 @@
         <v>105</v>
       </c>
       <c r="B104" s="4">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C104" s="4">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7118,10 +7150,10 @@
         <v>106</v>
       </c>
       <c r="B105" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C105" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7140,10 +7172,10 @@
         <v>108</v>
       </c>
       <c r="B107" s="4">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="C107" s="4">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7162,10 +7194,10 @@
         <v>110</v>
       </c>
       <c r="B109" s="4">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C109" s="4">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7173,10 +7205,10 @@
         <v>111</v>
       </c>
       <c r="B110" s="4">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C110" s="4">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7184,10 +7216,10 @@
         <v>112</v>
       </c>
       <c r="B111" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C111" s="4">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7195,10 +7227,10 @@
         <v>113</v>
       </c>
       <c r="B112" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C112" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7220,7 +7252,7 @@
         <v>4</v>
       </c>
       <c r="C114" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7228,10 +7260,10 @@
         <v>116</v>
       </c>
       <c r="B115" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C115" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7239,10 +7271,10 @@
         <v>117</v>
       </c>
       <c r="B116" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C116" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7272,10 +7304,10 @@
         <v>120</v>
       </c>
       <c r="B119" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C119" s="4">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7338,10 +7370,10 @@
         <v>126</v>
       </c>
       <c r="B125" s="4">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="C125" s="4">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7349,10 +7381,10 @@
         <v>127</v>
       </c>
       <c r="B126" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C126" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7371,7 +7403,7 @@
         <v>129</v>
       </c>
       <c r="B128" s="4">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C128" s="4">
         <v>50</v>
@@ -7382,10 +7414,10 @@
         <v>130</v>
       </c>
       <c r="B129" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C129" s="4">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7404,7 +7436,7 @@
         <v>132</v>
       </c>
       <c r="B131" s="4">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C131" s="4">
         <v>57</v>
@@ -7415,7 +7447,7 @@
         <v>133</v>
       </c>
       <c r="B132" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C132" s="4">
         <v>4</v>
@@ -7517,7 +7549,7 @@
         <v>7</v>
       </c>
       <c r="C141" s="4">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7528,7 +7560,7 @@
         <v>2</v>
       </c>
       <c r="C142" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7539,7 +7571,7 @@
         <v>2</v>
       </c>
       <c r="C143" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7580,10 +7612,10 @@
         <v>148</v>
       </c>
       <c r="B147" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C147" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7591,10 +7623,10 @@
         <v>149</v>
       </c>
       <c r="B148" s="4">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C148" s="4">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7602,10 +7634,10 @@
         <v>150</v>
       </c>
       <c r="B149" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C149" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7657,10 +7689,10 @@
         <v>155</v>
       </c>
       <c r="B154" s="4">
-        <v>283</v>
+        <v>294</v>
       </c>
       <c r="C154" s="4">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7668,7 +7700,7 @@
         <v>156</v>
       </c>
       <c r="B155" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C155" s="4">
         <v>0</v>
@@ -7690,10 +7722,10 @@
         <v>164</v>
       </c>
       <c r="B157" s="4">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C157" s="4">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7748,7 +7780,7 @@
         <v>1</v>
       </c>
       <c r="C162" s="4">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7756,10 +7788,10 @@
         <v>161</v>
       </c>
       <c r="B163" s="4">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C163" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7767,10 +7799,10 @@
         <v>162</v>
       </c>
       <c r="B164" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C164" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7781,7 +7813,7 @@
         <v>13</v>
       </c>
       <c r="C165" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7803,7 +7835,7 @@
         <v>30</v>
       </c>
       <c r="C167" s="4">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7855,10 +7887,10 @@
         <v>173</v>
       </c>
       <c r="B172" s="4">
-        <v>224</v>
+        <v>249</v>
       </c>
       <c r="C172" s="4">
-        <v>423</v>
+        <v>408</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7866,10 +7898,10 @@
         <v>174</v>
       </c>
       <c r="B173" s="4">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="C173" s="4">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7899,10 +7931,10 @@
         <v>177</v>
       </c>
       <c r="B176" s="4">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C176" s="4">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7913,7 +7945,7 @@
         <v>22</v>
       </c>
       <c r="C177" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7946,7 +7978,7 @@
         <v>73</v>
       </c>
       <c r="C180" s="4">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7957,7 +7989,7 @@
         <v>0</v>
       </c>
       <c r="C181" s="4">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -7976,7 +8008,7 @@
         <v>184</v>
       </c>
       <c r="B183" s="4">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C183" s="4">
         <v>27</v>
@@ -7998,10 +8030,10 @@
         <v>186</v>
       </c>
       <c r="B185" s="4">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C185" s="4">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8009,10 +8041,10 @@
         <v>187</v>
       </c>
       <c r="B186" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C186" s="4">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8023,7 +8055,7 @@
         <v>2</v>
       </c>
       <c r="C187" s="4">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8031,10 +8063,10 @@
         <v>189</v>
       </c>
       <c r="B188" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C188" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8053,10 +8085,10 @@
         <v>191</v>
       </c>
       <c r="B190" s="4">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="C190" s="4">
-        <v>787</v>
+        <v>834</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8086,10 +8118,10 @@
         <v>194</v>
       </c>
       <c r="B193" s="4">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C193" s="4">
-        <v>219</v>
+        <v>235</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8122,7 +8154,7 @@
         <v>1</v>
       </c>
       <c r="C196" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8166,7 +8198,7 @@
         <v>2</v>
       </c>
       <c r="C200" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8174,10 +8206,10 @@
         <v>202</v>
       </c>
       <c r="B201" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C201" s="4">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8199,7 +8231,7 @@
         <v>24</v>
       </c>
       <c r="C203" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="204" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8210,7 +8242,7 @@
         <v>1</v>
       </c>
       <c r="C204" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="205" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8240,7 +8272,7 @@
         <v>208</v>
       </c>
       <c r="B207" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C207" s="4">
         <v>6</v>
@@ -8287,7 +8319,7 @@
         <v>0</v>
       </c>
       <c r="C211" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8295,7 +8327,7 @@
         <v>213</v>
       </c>
       <c r="B212" s="4">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="C212" s="4">
         <v>70</v>
@@ -8306,7 +8338,7 @@
         <v>214</v>
       </c>
       <c r="B213" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C213" s="4">
         <v>11</v>
@@ -8317,10 +8349,10 @@
         <v>215</v>
       </c>
       <c r="B214" s="4">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C214" s="4">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8405,10 +8437,10 @@
         <v>223</v>
       </c>
       <c r="B222" s="4">
-        <v>654</v>
+        <v>682</v>
       </c>
       <c r="C222" s="4">
-        <v>1949</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8416,10 +8448,10 @@
         <v>224</v>
       </c>
       <c r="B223" s="4">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="C223" s="4">
-        <v>238</v>
+        <v>49</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8463,7 +8495,7 @@
         <v>10</v>
       </c>
       <c r="C227" s="4">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="228" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8471,10 +8503,10 @@
         <v>229</v>
       </c>
       <c r="B228" s="4">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C228" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="229" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8482,10 +8514,10 @@
         <v>230</v>
       </c>
       <c r="B229" s="4">
-        <v>617</v>
+        <v>659</v>
       </c>
       <c r="C229" s="4">
-        <v>1201</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8570,10 +8602,10 @@
         <v>238</v>
       </c>
       <c r="B237" s="4">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C237" s="4">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="238" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8581,10 +8613,10 @@
         <v>239</v>
       </c>
       <c r="B238" s="4">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="C238" s="4">
-        <v>224</v>
+        <v>203</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8592,10 +8624,10 @@
         <v>240</v>
       </c>
       <c r="B239" s="4">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C239" s="4">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="240" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8614,10 +8646,10 @@
         <v>242</v>
       </c>
       <c r="B241" s="4">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C241" s="4">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="242" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8625,10 +8657,10 @@
         <v>243</v>
       </c>
       <c r="B242" s="4">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="C242" s="4">
-        <v>229</v>
+        <v>211</v>
       </c>
     </row>
     <row r="243" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8683,7 +8715,7 @@
         <v>8</v>
       </c>
       <c r="C247" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="248" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8691,10 +8723,10 @@
         <v>249</v>
       </c>
       <c r="B248" s="4">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C248" s="4">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="249" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8702,10 +8734,10 @@
         <v>250</v>
       </c>
       <c r="B249" s="4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C249" s="4">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="250" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8724,10 +8756,10 @@
         <v>252</v>
       </c>
       <c r="B251" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C251" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="252" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -8786,11 +8818,11 @@
       </c>
     </row>
     <row r="258" spans="1:3" ht="130" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A258" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="B258" s="14"/>
-      <c r="C258" s="14"/>
+      <c r="A258" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="B258" s="13"/>
+      <c r="C258" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8803,13 +8835,450 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2:XFD2"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="11" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+    </row>
+    <row r="2" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>321</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>43925</v>
+      </c>
+      <c r="B3" s="15">
+        <v>9.3028117487000003E-2</v>
+      </c>
+      <c r="C3" s="7">
+        <v>63751</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>43926</v>
+      </c>
+      <c r="B4" s="15">
+        <v>0.11178618289999999</v>
+      </c>
+      <c r="C4" s="7">
+        <v>70938</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>43927</v>
+      </c>
+      <c r="B5" s="15">
+        <v>9.4582792398999999E-2</v>
+      </c>
+      <c r="C5" s="7">
+        <v>85357</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>43928</v>
+      </c>
+      <c r="B6" s="15">
+        <v>0.10455481467</v>
+      </c>
+      <c r="C6" s="7">
+        <v>88649</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>43929</v>
+      </c>
+      <c r="B7" s="15">
+        <v>0.10285438469000001</v>
+      </c>
+      <c r="C7" s="7">
+        <v>96258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>43930</v>
+      </c>
+      <c r="B8" s="15">
+        <v>9.7399245583000005E-2</v>
+      </c>
+      <c r="C8" s="7">
+        <v>106134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>43931</v>
+      </c>
+      <c r="B9" s="15">
+        <v>0.10656161941</v>
+      </c>
+      <c r="C9" s="7">
+        <v>115918</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>43932</v>
+      </c>
+      <c r="B10" s="15">
+        <v>0.11630204658</v>
+      </c>
+      <c r="C10" s="7">
+        <v>120533</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>43933</v>
+      </c>
+      <c r="B11" s="15">
+        <v>0.15846004693999999</v>
+      </c>
+      <c r="C11" s="7">
+        <v>124553</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>43934</v>
+      </c>
+      <c r="B12" s="15">
+        <v>0.12663481167000001</v>
+      </c>
+      <c r="C12" s="7">
+        <v>133226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>43935</v>
+      </c>
+      <c r="B13" s="15">
+        <v>0.10498117866999999</v>
+      </c>
+      <c r="C13" s="7">
+        <v>146467</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>43936</v>
+      </c>
+      <c r="B14" s="15">
+        <v>0.11520273229000001</v>
+      </c>
+      <c r="C14" s="7">
+        <v>151810</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>43937</v>
+      </c>
+      <c r="B15" s="15">
+        <v>0.11222407281000001</v>
+      </c>
+      <c r="C15" s="7">
+        <v>158547</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>43938</v>
+      </c>
+      <c r="B16" s="15">
+        <v>9.8157255677999988E-2</v>
+      </c>
+      <c r="C16" s="7">
+        <v>169536</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>43939</v>
+      </c>
+      <c r="B17" s="15">
+        <v>9.2404132647000009E-2</v>
+      </c>
+      <c r="C17" s="7">
+        <v>176239</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>43940</v>
+      </c>
+      <c r="B18" s="15">
+        <v>0.10138630668</v>
+      </c>
+      <c r="C18" s="7">
+        <v>182710</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>43941</v>
+      </c>
+      <c r="B19" s="15">
+        <v>0.11004621304000001</v>
+      </c>
+      <c r="C19" s="7">
+        <v>190394</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>43942</v>
+      </c>
+      <c r="B20" s="15">
+        <v>8.7779208420000004E-2</v>
+      </c>
+      <c r="C20" s="7">
+        <v>205399</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>43943</v>
+      </c>
+      <c r="B21" s="15">
+        <v>7.9229342674999995E-2</v>
+      </c>
+      <c r="C21" s="7">
+        <v>216783</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>43944</v>
+      </c>
+      <c r="B22" s="15">
+        <v>8.2334089517999989E-2</v>
+      </c>
+      <c r="C22" s="7">
+        <v>225078</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>43945</v>
+      </c>
+      <c r="B23" s="15">
+        <v>6.8558846595E-2</v>
+      </c>
+      <c r="C23" s="7">
+        <v>242547</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>43946</v>
+      </c>
+      <c r="B24" s="15">
+        <v>6.0544778169000002E-2</v>
+      </c>
+      <c r="C24" s="7">
+        <v>262816</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>43947</v>
+      </c>
+      <c r="B25" s="15">
+        <v>6.0413187428999995E-2</v>
+      </c>
+      <c r="C25" s="7">
+        <v>276021</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>43948</v>
+      </c>
+      <c r="B26" s="15">
+        <v>5.9928569749999994E-2</v>
+      </c>
+      <c r="C26" s="7">
+        <v>290517</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>43949</v>
+      </c>
+      <c r="B27" s="15">
+        <v>6.1027978133999995E-2</v>
+      </c>
+      <c r="C27" s="7">
+        <v>300384</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>43950</v>
+      </c>
+      <c r="B28" s="15">
+        <v>5.6960049937999996E-2</v>
+      </c>
+      <c r="C28" s="7">
+        <v>314790</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>43951</v>
+      </c>
+      <c r="B29" s="15">
+        <v>6.0180278737000006E-2</v>
+      </c>
+      <c r="C29" s="7">
+        <v>330300</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>43952</v>
+      </c>
+      <c r="B30" s="15">
+        <v>6.1331624681000001E-2</v>
+      </c>
+      <c r="C30" s="7">
+        <v>351775</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>43953</v>
+      </c>
+      <c r="B31" s="15">
+        <v>5.6304777925000001E-2</v>
+      </c>
+      <c r="C31" s="7">
+        <v>380648</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>43954</v>
+      </c>
+      <c r="B32" s="15">
+        <v>6.2483132253000007E-2</v>
+      </c>
+      <c r="C32" s="7">
+        <v>390560</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>43955</v>
+      </c>
+      <c r="B33" s="15">
+        <v>5.7571906479999997E-2</v>
+      </c>
+      <c r="C33" s="7">
+        <v>407398</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>43956</v>
+      </c>
+      <c r="B34" s="15">
+        <v>5.6173278776E-2</v>
+      </c>
+      <c r="C34" s="7">
+        <v>427210</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <v>43957</v>
+      </c>
+      <c r="B35" s="15">
+        <v>5.8312929177999996E-2</v>
+      </c>
+      <c r="C35" s="7">
+        <v>438938</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <v>43958</v>
+      </c>
+      <c r="B36" s="15">
+        <v>5.8488571382999996E-2</v>
+      </c>
+      <c r="C36" s="7">
+        <v>455162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
+        <v>43959</v>
+      </c>
+      <c r="B37" s="15">
+        <v>5.8878437566999994E-2</v>
+      </c>
+      <c r="C37" s="7">
+        <v>477118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A39:C39"/>
+  </mergeCells>
+  <pageMargins left="0.05" right="0.05" top="0.5" bottom="0.5" header="0" footer="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8819,468 +9288,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="B1" s="14"/>
+      <c r="A1" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B3" s="7">
-        <v>14661</v>
+        <v>15470</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B4" s="7">
-        <v>440501</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>276</v>
-      </c>
-      <c r="B6" s="14"/>
+        <v>461648</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B5" s="7">
+        <v>477118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="B7" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.05" right="0.05" top="0.5" bottom="0.5" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C36"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-    </row>
-    <row r="2" spans="1:3" ht="58" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>43925</v>
-      </c>
-      <c r="B3" s="11">
-        <v>9.3028117486999999</v>
-      </c>
-      <c r="C3" s="7">
-        <v>63751</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>43926</v>
-      </c>
-      <c r="B4" s="11">
-        <v>11.178618289999999</v>
-      </c>
-      <c r="C4" s="7">
-        <v>70938</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>43927</v>
-      </c>
-      <c r="B5" s="11">
-        <v>9.4582792398999995</v>
-      </c>
-      <c r="C5" s="7">
-        <v>85357</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>43928</v>
-      </c>
-      <c r="B6" s="11">
-        <v>10.455481467</v>
-      </c>
-      <c r="C6" s="7">
-        <v>88649</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>43929</v>
-      </c>
-      <c r="B7" s="11">
-        <v>10.285438469000001</v>
-      </c>
-      <c r="C7" s="7">
-        <v>96258</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>43930</v>
-      </c>
-      <c r="B8" s="11">
-        <v>9.7399245583000003</v>
-      </c>
-      <c r="C8" s="7">
-        <v>106134</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>43931</v>
-      </c>
-      <c r="B9" s="11">
-        <v>10.656161941000001</v>
-      </c>
-      <c r="C9" s="7">
-        <v>115918</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>43932</v>
-      </c>
-      <c r="B10" s="11">
-        <v>11.630204658</v>
-      </c>
-      <c r="C10" s="7">
-        <v>120533</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>43933</v>
-      </c>
-      <c r="B11" s="11">
-        <v>15.846004693999999</v>
-      </c>
-      <c r="C11" s="7">
-        <v>124553</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>43934</v>
-      </c>
-      <c r="B12" s="11">
-        <v>12.663481167</v>
-      </c>
-      <c r="C12" s="7">
-        <v>133226</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>43935</v>
-      </c>
-      <c r="B13" s="11">
-        <v>10.498117866999999</v>
-      </c>
-      <c r="C13" s="7">
-        <v>146467</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>43936</v>
-      </c>
-      <c r="B14" s="11">
-        <v>11.520273229000001</v>
-      </c>
-      <c r="C14" s="7">
-        <v>151810</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <v>43937</v>
-      </c>
-      <c r="B15" s="11">
-        <v>11.222407281000001</v>
-      </c>
-      <c r="C15" s="7">
-        <v>158547</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
-        <v>43938</v>
-      </c>
-      <c r="B16" s="11">
-        <v>9.8157255677999995</v>
-      </c>
-      <c r="C16" s="7">
-        <v>169536</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <v>43939</v>
-      </c>
-      <c r="B17" s="11">
-        <v>9.2404132647000008</v>
-      </c>
-      <c r="C17" s="7">
-        <v>176239</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <v>43940</v>
-      </c>
-      <c r="B18" s="11">
-        <v>10.138630667999999</v>
-      </c>
-      <c r="C18" s="7">
-        <v>182710</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
-        <v>43941</v>
-      </c>
-      <c r="B19" s="11">
-        <v>11.004621304</v>
-      </c>
-      <c r="C19" s="7">
-        <v>190394</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
-        <v>43942</v>
-      </c>
-      <c r="B20" s="11">
-        <v>8.7779208420000003</v>
-      </c>
-      <c r="C20" s="7">
-        <v>205399</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <v>43943</v>
-      </c>
-      <c r="B21" s="11">
-        <v>7.9229342674999996</v>
-      </c>
-      <c r="C21" s="7">
-        <v>216783</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
-        <v>43944</v>
-      </c>
-      <c r="B22" s="11">
-        <v>8.2334089517999995</v>
-      </c>
-      <c r="C22" s="7">
-        <v>225078</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
-        <v>43945</v>
-      </c>
-      <c r="B23" s="11">
-        <v>6.8558846595</v>
-      </c>
-      <c r="C23" s="7">
-        <v>242547</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
-        <v>43946</v>
-      </c>
-      <c r="B24" s="11">
-        <v>6.0544778169000004</v>
-      </c>
-      <c r="C24" s="7">
-        <v>262816</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
-        <v>43947</v>
-      </c>
-      <c r="B25" s="11">
-        <v>6.0413187428999997</v>
-      </c>
-      <c r="C25" s="7">
-        <v>276021</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
-        <v>43948</v>
-      </c>
-      <c r="B26" s="11">
-        <v>5.9928569749999996</v>
-      </c>
-      <c r="C26" s="7">
-        <v>290517</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
-        <v>43949</v>
-      </c>
-      <c r="B27" s="11">
-        <v>6.1027978133999996</v>
-      </c>
-      <c r="C27" s="7">
-        <v>300384</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
-        <v>43950</v>
-      </c>
-      <c r="B28" s="11">
-        <v>5.6960049937999999</v>
-      </c>
-      <c r="C28" s="7">
-        <v>314790</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
-        <v>43951</v>
-      </c>
-      <c r="B29" s="11">
-        <v>6.0180278737000004</v>
-      </c>
-      <c r="C29" s="7">
-        <v>330300</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6">
-        <v>43952</v>
-      </c>
-      <c r="B30" s="11">
-        <v>6.1331624681000001</v>
-      </c>
-      <c r="C30" s="7">
-        <v>351775</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
-        <v>43953</v>
-      </c>
-      <c r="B31" s="11">
-        <v>5.6304777924999998</v>
-      </c>
-      <c r="C31" s="7">
-        <v>380648</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6">
-        <v>43954</v>
-      </c>
-      <c r="B32" s="11">
-        <v>6.2483132253000004</v>
-      </c>
-      <c r="C32" s="7">
-        <v>390560</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
-        <v>43955</v>
-      </c>
-      <c r="B33" s="11">
-        <v>5.7571906479999999</v>
-      </c>
-      <c r="C33" s="7">
-        <v>407398</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6">
-        <v>43956</v>
-      </c>
-      <c r="B34" s="11">
-        <v>5.6173278776000002</v>
-      </c>
-      <c r="C34" s="7">
-        <v>427210</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6">
-        <v>43957</v>
-      </c>
-      <c r="B35" s="11">
-        <v>5.8312929177999999</v>
-      </c>
-      <c r="C35" s="7">
-        <v>438938</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6">
-        <v>43958</v>
-      </c>
-      <c r="B36" s="11">
-        <v>5.8488571382999996</v>
-      </c>
-      <c r="C36" s="7">
-        <v>455162</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.05" right="0.05" top="0.5" bottom="0.5" header="0" footer="0"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>Tests include those performed by public labs (Laboratory Response Network) and private labs (commercial labs, hospitals, physician offices, and drive-thru sites) reported electronically and non-electronically to DSHS.</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
 
@@ -9301,64 +9358,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>277</v>
-      </c>
-      <c r="B1" s="14"/>
+      <c r="A1" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B3" s="7">
-        <v>1750</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B4" s="7">
-        <v>56624</v>
+        <v>56186</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B5" s="7">
-        <v>17902</v>
+        <v>17670</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B6" s="7">
-        <v>1959</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B7" s="7">
-        <v>6494</v>
+        <v>6131</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>276</v>
-      </c>
-      <c r="B9" s="14"/>
+      <c r="A9" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="B9" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -9377,188 +9434,188 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2:XFD2"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3:C16"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="A1" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B3" s="9">
-        <v>32</v>
-      </c>
-      <c r="C3" s="12">
+        <v>33</v>
+      </c>
+      <c r="C3" s="15">
         <f>B3/B$16</f>
-        <v>2.5532593951966809E-3</v>
+        <v>2.5527964724994198E-3</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B4" s="9">
-        <v>141</v>
-      </c>
-      <c r="C4" s="12">
+        <v>147</v>
+      </c>
+      <c r="C4" s="15">
         <f t="shared" ref="C4:C16" si="0">B4/B$16</f>
-        <v>1.1250299210085375E-2</v>
+        <v>1.1371547922951961E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B5" s="9">
-        <v>376</v>
-      </c>
-      <c r="C5" s="12">
+        <v>388</v>
+      </c>
+      <c r="C5" s="15">
         <f t="shared" si="0"/>
-        <v>3.0000797893560999E-2</v>
+        <v>3.0014697919084087E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B6" s="9">
-        <v>1952</v>
-      </c>
-      <c r="C6" s="12">
+        <v>2006</v>
+      </c>
+      <c r="C6" s="15">
         <f t="shared" si="0"/>
-        <v>0.15574882310699753</v>
+        <v>0.15517908254041929</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B7" s="9">
-        <v>2275</v>
-      </c>
-      <c r="C7" s="12">
+        <v>2346</v>
+      </c>
+      <c r="C7" s="15">
         <f t="shared" si="0"/>
-        <v>0.18152078512726402</v>
+        <v>0.18148062195404965</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B8" s="9">
-        <v>2369</v>
-      </c>
-      <c r="C8" s="12">
+        <v>2448</v>
+      </c>
+      <c r="C8" s="15">
         <f t="shared" si="0"/>
-        <v>0.18902098460065428</v>
+        <v>0.18937108377813877</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B9" s="9">
-        <v>2297</v>
-      </c>
-      <c r="C9" s="12">
+        <v>2379</v>
+      </c>
+      <c r="C9" s="15">
         <f t="shared" si="0"/>
-        <v>0.18327615096146174</v>
+        <v>0.18403341842654908</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B10" s="9">
-        <v>955</v>
-      </c>
-      <c r="C10" s="12">
+        <v>993</v>
+      </c>
+      <c r="C10" s="15">
         <f t="shared" si="0"/>
-        <v>7.6198835075400942E-2</v>
+        <v>7.6815966581573455E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B11" s="9">
-        <v>697</v>
-      </c>
-      <c r="C11" s="12">
+        <v>724</v>
+      </c>
+      <c r="C11" s="15">
         <f t="shared" si="0"/>
-        <v>5.5613181201627705E-2</v>
+        <v>5.6006807457259999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="B12" s="9">
-        <v>477</v>
-      </c>
-      <c r="C12" s="12">
+        <v>491</v>
+      </c>
+      <c r="C12" s="15">
         <f t="shared" si="0"/>
-        <v>3.8059522859650523E-2</v>
+        <v>3.7982517212036819E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="B13" s="9">
-        <v>325</v>
-      </c>
-      <c r="C13" s="12">
+        <v>330</v>
+      </c>
+      <c r="C13" s="15">
         <f t="shared" si="0"/>
-        <v>2.5931540732466288E-2</v>
+        <v>2.5527964724994197E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B14" s="9">
-        <v>596</v>
-      </c>
-      <c r="C14" s="12">
+        <v>601</v>
+      </c>
+      <c r="C14" s="15">
         <f t="shared" si="0"/>
-        <v>4.7554456235538181E-2</v>
+        <v>4.6491838787034889E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B15" s="9">
         <v>41</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="15">
         <f t="shared" si="0"/>
-        <v>3.2713636000957472E-3</v>
+        <v>3.1716562234083701E-3</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -9566,26 +9623,26 @@
         <v>258</v>
       </c>
       <c r="B16" s="9">
-        <v>12533</v>
-      </c>
-      <c r="C16" s="12">
+        <v>12927</v>
+      </c>
+      <c r="C16" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
-        <v>301</v>
-      </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
+      <c r="A18" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
     </row>
     <row r="19" spans="1:3" ht="43" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
+      <c r="A19" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -9594,7 +9651,7 @@
     <mergeCell ref="A19:C19"/>
   </mergeCells>
   <pageMargins left="0.05" right="0.05" top="0.5" bottom="0.5" header="0" footer="0"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -9605,7 +9662,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2:XFD2"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9616,57 +9673,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="A1" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B3" s="9">
-        <v>6014</v>
-      </c>
-      <c r="C3" s="12">
+        <v>6136</v>
+      </c>
+      <c r="C3" s="15">
         <f>B3/B$6</f>
-        <v>0.47985318758477619</v>
+        <v>0.47466542894716485</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="B4" s="9">
-        <v>6252</v>
-      </c>
-      <c r="C4" s="12">
+        <v>6520</v>
+      </c>
+      <c r="C4" s="15">
         <f t="shared" ref="C4:C6" si="0">B4/B$6</f>
-        <v>0.49884305433655152</v>
+        <v>0.50437069699079451</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B5" s="9">
-        <v>267</v>
-      </c>
-      <c r="C5" s="12">
+        <v>271</v>
+      </c>
+      <c r="C5" s="15">
         <f t="shared" si="0"/>
-        <v>2.1303758078672304E-2</v>
+        <v>2.0963874062040689E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.25">
@@ -9674,26 +9731,26 @@
         <v>258</v>
       </c>
       <c r="B6" s="9">
-        <v>12533</v>
-      </c>
-      <c r="C6" s="12">
+        <v>12927</v>
+      </c>
+      <c r="C6" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>301</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
+      <c r="A8" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
     </row>
     <row r="9" spans="1:3" ht="43" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
+      <c r="A9" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>